<commit_message>
Project Status Update + Gif Generation
</commit_message>
<xml_diff>
--- a/simulation_results_I.xlsx
+++ b/simulation_results_I.xlsx
@@ -5,22 +5,35 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://office365stanford-my.sharepoint.com/personal/datsimp_stanford_edu/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://office365stanford-my.sharepoint.com/personal/datsimp_stanford_edu/Documents/Stanford/AA228V/Final Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB685CA8-959C-4AC6-8235-3F9B1AC19232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{AB685CA8-959C-4AC6-8235-3F9B1AC19232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38258E63-ACE5-4300-A9B0-3BB4A00FFC23}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{48F81B54-F06A-4CBE-991E-C7E2B326AACC}"/>
   </bookViews>
   <sheets>
     <sheet name="simulation_results" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="10">
   <si>
     <t>Trial #</t>
   </si>
@@ -47,6 +60,9 @@
   </si>
   <si>
     <t>Drones got Stuck</t>
+  </si>
+  <si>
+    <t>p_nobudget</t>
   </si>
 </sst>
 </file>
@@ -907,10 +923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E35E950B-F78B-4088-8F7E-04F14F25FCA7}">
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -918,7 +934,7 @@
     <col min="2" max="2" width="43.3828125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -935,7 +951,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -951,8 +967,11 @@
       <c r="E2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -968,8 +987,12 @@
       <c r="E3">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="H3">
+        <f>COUNTIF(B:B, "Drones got Stuck") / (COUNTA(B:B) - 1)</f>
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -986,7 +1009,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1003,7 +1026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1020,7 +1043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1037,7 +1060,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1054,7 +1077,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1071,7 +1094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1088,7 +1111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1105,7 +1128,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1122,7 +1145,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1139,7 +1162,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1156,7 +1179,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1173,7 +1196,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>